<commit_message>
Ejecutar Codigo desde Excel
</commit_message>
<xml_diff>
--- a/COMPARAR_PRECIOS.xlsx
+++ b/COMPARAR_PRECIOS.xlsx
@@ -274,14 +274,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -289,7 +289,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -298,7 +298,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
@@ -870,9 +870,9 @@
   </sheetPr>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
+      <selection pane="bottomLeft" activeCell="L32" sqref="L32:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1360,13 +1360,13 @@
       <c r="B13" s="27" t="n"/>
       <c r="C13" s="27" t="n"/>
       <c r="D13" s="28" t="n"/>
-      <c r="G13" s="29" t="inlineStr">
+      <c r="G13" s="32" t="inlineStr">
         <is>
           <t>TEJIDO</t>
         </is>
       </c>
       <c r="H13" s="28" t="n"/>
-      <c r="K13" s="29" t="inlineStr">
+      <c r="K13" s="32" t="inlineStr">
         <is>
           <t>TEJIDO</t>
         </is>
@@ -1691,13 +1691,13 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="27" t="n"/>
       <c r="D22" s="28" t="n"/>
-      <c r="G22" s="32" t="inlineStr">
+      <c r="G22" s="29" t="inlineStr">
         <is>
           <t>PUERTA/PORTON</t>
         </is>
       </c>
       <c r="H22" s="28" t="n"/>
-      <c r="K22" s="32" t="inlineStr">
+      <c r="K22" s="29" t="inlineStr">
         <is>
           <t>PUERTA/PORTON</t>
         </is>
@@ -1945,13 +1945,13 @@
       <c r="B31" s="27" t="n"/>
       <c r="C31" s="27" t="n"/>
       <c r="D31" s="28" t="n"/>
-      <c r="G31" s="29" t="inlineStr">
+      <c r="G31" s="32" t="inlineStr">
         <is>
           <t>PUA</t>
         </is>
       </c>
       <c r="H31" s="28" t="n"/>
-      <c r="K31" s="29" t="inlineStr">
+      <c r="K31" s="32" t="inlineStr">
         <is>
           <t>PUA</t>
         </is>
@@ -2050,15 +2050,15 @@
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="G31:H31"/>
     <mergeCell ref="K31:L31"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A1:B1"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="G3:H3"/>

</xml_diff>